<commit_message>
updated requirement tracebility matrix
</commit_message>
<xml_diff>
--- a/dev_multimodel_category/docs/Requirement Traceability Matrix.xlsx
+++ b/dev_multimodel_category/docs/Requirement Traceability Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="143">
   <si>
     <t>Iteration 1 Requirement Traceability Matrix</t>
   </si>
@@ -980,6 +980,547 @@
   </si>
   <si>
     <t xml:space="preserve">Exception Handling </t>
+  </si>
+  <si>
+    <t>Iteration 4 Requirement Traceability Matrix</t>
+  </si>
+  <si>
+    <t>Supporting caTissueSuite</t>
+  </si>
+  <si>
+    <t>User manual</t>
+  </si>
+  <si>
+    <t>Optimizations for retrieveing data and viewing results: Part 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Java:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+AbstractQueryResultTransformer.java (M1)
+QueryExecutor.java (M1)
+QueryExecutorThreadPool.java (M1)
+QueryOperations.java (M3)
+SearchQueryExecutor.java (M3)
+SpreadSheetResultTransformer.java (M3)
+ExecuteQueryBizLogic.java (M3)
+ExecuteQueryAction.java (M3)
+ExportDataAction.java (M3)
+KeywordSearchAction.java (M3)
+PreExecuteQueryAction.java (M3)
+TransformQueryResultsAction.java (M3)
+CategoryToSpreadsheetTransformer.java (M3)
+QueryExecutorPropertes.java (M1)
+TransformedResultObjectWithContactInfo.java (M3)
+HomeAction.java (M3)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>JSP:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+addlimit.jsp (M3)
+searchresults.jsp (M3)
+searchresultspanel.jsp (M3)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Style Sheets:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+searchresults.css (M3)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Java Scripts:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+ajax.js (M3)</t>
+    </r>
+  </si>
+  <si>
+    <t>8842, 8846, 8840, 9259, 9260, 9261, 8839, 8841, 8843, 8844, 8845, 8850, 9049, 9050, 9051, 9052, 9053, 9054, 9055, 9056, 9057, 9058 ,9059, 9060</t>
+  </si>
+  <si>
+    <t>Create-save multi model category from backend</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Java</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:
+ MultiModelCategoryXMLParser.java
+MultiModelCategoryXMLParser.java
+MMCQueryExecutionHandler.java, MMCQueryResultConflator.java, MultimodelCategoryQueryPreprocessor.java (M1)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Test Cases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: 
+MultiModelCategoryXMLParserTest.javaJava: 
+MultiModelCategoryXMLParserTest.java</t>
+    </r>
+  </si>
+  <si>
+    <t>Save form-query using multi-model category</t>
+  </si>
+  <si>
+    <t>Java: MultimodelCategoryQueryProcessor.java (M1)</t>
+  </si>
+  <si>
+    <t>Execute query created using multi-model category</t>
+  </si>
+  <si>
+    <t>Java: MultimodelCategoryQueryPreprocessor.java (M1)</t>
+  </si>
+  <si>
+    <t>9799, 9800, 9802, 9804, 9805, 9806, 9807,9808</t>
+  </si>
+  <si>
+    <t>QA cycle on v3.0 (all 3 iterations)</t>
+  </si>
+  <si>
+    <t>Items required for 3.0 release- deployment, etc.</t>
+  </si>
+  <si>
+    <t>Release related activity</t>
+  </si>
+  <si>
+    <t>Iteration 4 QA cycle</t>
+  </si>
+  <si>
+    <t>Performance testing and improvements : caB2B Iteration 3.0 activity</t>
+  </si>
+  <si>
+    <t>Iteration 5 Requirement Traceability Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NxM rows display for keyword and form based query </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Java: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>QueryBizLogic.java(M3)
+KeywordQueryExecutionHandler.java(M3)
+CaB2BQueryExecutionHandler.java(M1)
+MMCQueryExecutionHandler.java(M1)
+QueryExecutionHandler.java(M1)
+ExecuteQueryAction.java(M3)
+TransformQueryResultsAction.java(M3)
+PreExecuteQueryAction.java(M3)
+QueryExecutor.java(M1)
+QueryExecutorUtil.java(M1)
+SavedQueryBizLogic.java(M3)
+HomeAction.java (M3)
+TransformedResultObjectWithContactInfo.java (M3)
+CategoryToSpreadsheetTransformer.java (M3)
+QueryExecutorPropertes.java (M1)
+SpreadSheetResultTransformer.java (M3)
+AbstractQueryResultTransformer.java (M1)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+JSP: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>searchresults.jsp
+searchresultspanel.jsp
+home.jsp</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Java Script: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ajax.js</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Stylesheets: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+common.css
+searchresults.css</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Showing MMC results in single spreadsheet </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Showing Permissible Values in MMC based form query </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiding system generated artifacts created as part of MMC </t>
+  </si>
+  <si>
+    <t>9897                 9898
+9806</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Execute in background </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Java</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: 
+DisplayDashboardAction.java, BackgroundQueryAction.java, ExportResultsAction.java, QueryStatusDVO.java, QueryConditionsDVO.java
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>JSP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: 
+dashboard.jsp, dashboardpanel.jsp
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Java Script</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">: 
+ajax.js, jquery.js
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Stylesheets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: 
+dashboard.css, common.css</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">9862            9863  9864            9865  9866            9867  9868            9869  9870            9871  9872            9873  9874            9875  9876            9877  9878            9879  9880            9881  9882            9883  9884            9885  9886            9887  9888            9889  9890            9891  9892            9893  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.0 deployment activities and overheads </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For keyword query show 100 records (including NxM) </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Java: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+QueryBizLogic.java(M3)
+KeywordQueryExecutionHandler.java(M3)
+QueryExecutionHandler.java(M1)
+ExecuteQueryAction.java(M3)
+TransformQueryResultsAction.java(M3)
+PreExecuteQueryAction.java(M3)
+QueryExecutor.java(M1)
+QueryExecutorUtil.java(M1)
+SavedQueryBizLogic.java(M3)
+HomeAction.java (M3)
+TransformedResultObjectWithContactInfo.java (M3)
+CategoryToSpreadsheetTransformer.java (M3)
+QueryExecutorPropertes.java (M1)
+SpreadSheetResultTransformer.java (M3)
+AbstractQueryResultTransformer.java (M1)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">JSP: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+searchresults.jsp
+searchresultspanel.jsp
+home.jsp
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Java Script: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+ajax.js
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Stylesheets: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+common.css
+searchresults.css</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Running thick client on https </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyword query using multi model category  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigation : client over HTTP &amp; web app over HTTPS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Configuration in Jboss server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA cycle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Testing related activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database migration 3.0 to 3.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation for 3.1 release  </t>
+  </si>
+  <si>
+    <t>Auditing feature analysis</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1614,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1096,6 +1637,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1104,10 +1654,9 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1137,7 +1686,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1152,6 +1700,21 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1448,881 +2011,1306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="66.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="16" customWidth="1"/>
     <col min="4" max="4" width="57.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="26.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="60.75">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>375</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="24.75">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>376</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>377</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="24.75">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>378</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="24.75">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>379</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="48.75">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>380</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="36.75">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>381</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="36.75">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>382</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="96.75">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>383</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>7589</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="48.75">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>474</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="16.5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="26.25">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="204.75">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>475</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="144.75">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>569</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="108.75">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>479</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="108.75">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>476</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="96.75">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>480</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>562</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>481</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="36.75">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>635</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="36.75">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>478</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>740</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="5"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>565</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="5"/>
+      <c r="E27" s="4"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" ht="24.75">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>483</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="4"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="16.5">
-      <c r="A31" s="1"/>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" ht="26.25">
-      <c r="A32" s="19" t="s">
+      <c r="A32" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="18" t="s">
         <v>5</v>
       </c>
       <c r="F32" s="1"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>637</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="4"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="24.75">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>1654</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E34" s="5"/>
+      <c r="E34" s="4"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="24.75">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>1060</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="48.75">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>567</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="13"/>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="60.75">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>571</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="4">
         <v>7994</v>
       </c>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>1059</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="15"/>
+      <c r="E38" s="13"/>
       <c r="F38" s="1"/>
     </row>
     <row r="39" spans="1:6" ht="24.75">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>1057</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="13"/>
       <c r="F39" s="1"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>1063</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="15"/>
+      <c r="E40" s="13"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>1395</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="15"/>
+      <c r="E41" s="13"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>1062</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E42" s="15"/>
+      <c r="E42" s="13"/>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>1388</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E43" s="15"/>
+      <c r="E43" s="13"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>633</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E44" s="15"/>
+      <c r="E44" s="13"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" ht="24.75">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>1655</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="15"/>
+      <c r="E45" s="13"/>
       <c r="F45" s="1"/>
     </row>
     <row r="46" spans="1:6" ht="24.75">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>1392</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E46" s="15"/>
+      <c r="E46" s="13"/>
       <c r="F46" s="1"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
+      <c r="C47" s="2"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="3"/>
+      <c r="E47" s="2"/>
       <c r="F47" s="1"/>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="1"/>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="1"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" ht="16.5">
+      <c r="A49" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" ht="26.25">
+      <c r="A50" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51">
+        <v>2545</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="3">
+        <v>1062</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53">
+        <v>2542</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" ht="336.75">
+      <c r="A54">
+        <v>1391</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" s="4"/>
+      <c r="D54" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" ht="96">
+      <c r="A55" s="3">
+        <v>564</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="3">
+        <v>631</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E56" s="13"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" ht="43.5">
+      <c r="A57" s="3">
+        <v>1396</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58">
+        <v>2322</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="13"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59">
+        <v>2323</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C59" s="4"/>
+      <c r="D59" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E59" s="13"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="3">
+        <v>2327</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="13"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="3">
+        <v>3060</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="10"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="10"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" ht="16.5">
+      <c r="A64" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:5" ht="26.25">
+      <c r="A65" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="360.75">
+      <c r="A66" s="3">
+        <v>3068</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E66" s="4"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="3">
+        <v>3433</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C67" s="4"/>
+      <c r="D67" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E67" s="4"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="3">
+        <v>3437</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="13"/>
+    </row>
+    <row r="69" spans="1:5" ht="24.75">
+      <c r="A69" s="3">
+        <v>3434</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C69" s="4"/>
+      <c r="D69" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E69" s="23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="228.75">
+      <c r="A70" s="3">
+        <v>3067</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="3">
+        <v>3435</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" s="4"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="13"/>
+    </row>
+    <row r="72" spans="1:5" ht="336.75">
+      <c r="A72" s="3">
+        <v>3436</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E72" s="13"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="3">
+        <v>3061</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" s="4"/>
+      <c r="D73" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E73" s="13"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="3">
+        <v>3439</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="13"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="3">
+        <v>3062</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" s="4"/>
+      <c r="D75" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E75" s="13"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="3">
+        <v>3440</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E76" s="13"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="3">
+        <v>3441</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C77" s="4"/>
+      <c r="D77" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E77" s="13"/>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="3">
+        <v>3442</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="13"/>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="3">
+        <v>3478</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="13"/>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="10"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="22"/>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="10"/>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="22"/>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="10"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="22"/>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="1"/>
+      <c r="B83" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="1"/>
-      <c r="B49" s="17" t="s">
+      <c r="C83" s="2"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="1"/>
+      <c r="B84" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="1"/>
-      <c r="B50" s="17" t="s">
+      <c r="C84" s="2"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="1"/>
+      <c r="B85" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="1"/>
-    </row>
-    <row r="62" spans="1:6">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="1"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="1"/>
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="1"/>
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="1"/>
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="1"/>
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="1"/>
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="1"/>
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A64:E64"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>